<commit_message>
boyut için excelden veri yükleme
</commit_message>
<xml_diff>
--- a/Wms12m.Presentation/Content/SizeSablon.xlsx
+++ b/Wms12m.Presentation/Content/SizeSablon.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9615"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,24 +24,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>MalKodu</t>
-  </si>
-  <si>
-    <t>Miktar</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Birim</t>
+  </si>
+  <si>
+    <t>Mal Kodu</t>
+  </si>
+  <si>
+    <t>En</t>
+  </si>
+  <si>
+    <t>Boy</t>
+  </si>
+  <si>
+    <t>Derinlik</t>
+  </si>
+  <si>
+    <t>Ağırlık</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;₺&quot;"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -75,7 +81,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -83,20 +89,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,33 +400,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="sZA3Sn8yyBF/TvhJIiDhOPmnaQ8Z32hPYdnC803xpiljlql7SGQ+TJWTng8X0MdJ69aOZYzduqc5Nf+vstWcig==" saltValue="uJK2kr7tOuwluac27JmZ/g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ize56jtEYfp/7a9kqLd+WYphwGomN1O2YMVDxUrjfj38pFfsRf1PWiKbGk+4TDqnTpq+7azPBn2aojzxpgTkdQ==" saltValue="TRki5xUcrBsUN9ui3mb8ug==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>